<commit_message>
local search(max-cut) : get avg no. of iterations and avg cut-value via global variables
</commit_message>
<xml_diff>
--- a/asgn-3-local-search/stats_local_search.xlsx
+++ b/asgn-3-local-search/stats_local_search.xlsx
@@ -436,7 +436,7 @@
   <dimension ref="D7:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,25 +515,25 @@
         <v>1600</v>
       </c>
       <c r="G11">
-        <v>444</v>
+        <v>460</v>
       </c>
       <c r="H11">
-        <v>432</v>
+        <v>464</v>
       </c>
       <c r="I11">
-        <v>424</v>
+        <v>492</v>
       </c>
       <c r="J11">
-        <v>2.6</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="K11">
-        <v>466.2</v>
+        <v>464.4</v>
       </c>
       <c r="L11">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M11">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="N11">
         <v>627</v>
@@ -550,25 +550,25 @@
         <v>1600</v>
       </c>
       <c r="G12">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="H12">
-        <v>432</v>
+        <v>468</v>
       </c>
       <c r="I12">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="J12">
-        <v>3.04</v>
+        <v>3</v>
       </c>
       <c r="K12">
-        <v>449.04</v>
+        <v>477.2</v>
       </c>
       <c r="L12">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M12">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="N12">
         <v>645</v>
@@ -585,26 +585,12 @@
         <v>1600</v>
       </c>
       <c r="G13">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="H13">
-        <v>464</v>
-      </c>
-      <c r="I13">
-        <v>472</v>
-      </c>
-      <c r="J13" s="1">
-        <v>3.56</v>
-      </c>
-      <c r="K13">
-        <v>426.72</v>
-      </c>
-      <c r="L13">
-        <v>10</v>
-      </c>
-      <c r="M13">
-        <v>472</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="J13" s="1"/>
       <c r="N13">
         <v>621</v>
       </c>
@@ -618,6 +604,30 @@
       </c>
       <c r="F14">
         <v>4661</v>
+      </c>
+      <c r="G14">
+        <v>2922</v>
+      </c>
+      <c r="H14">
+        <v>2934</v>
+      </c>
+      <c r="I14">
+        <v>2958</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>2934</v>
+      </c>
+      <c r="L14">
+        <v>30</v>
+      </c>
+      <c r="M14">
+        <v>2958</v>
+      </c>
+      <c r="N14">
+        <v>3169</v>
       </c>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.3">

</xml_diff>